<commit_message>
Files updated for FV function documentation.
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/FV.xlsx
+++ b/xlsx/tests/docs/FV.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\Function descriptions\FV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FC729A-6FC1-4226-B328-4D36184339E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA86FDDE-66C0-408B-A578-B826CC7F1956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{485CA009-6F4A-460D-891C-D7B8869F48AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>rate</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Future Value</t>
+  </si>
+  <si>
+    <t>Formula Text</t>
   </si>
 </sst>
 </file>
@@ -478,19 +481,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698A441E-9203-46F3-91E3-D681B30E39C3}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,8 +513,11 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>0.05</v>
       </c>
@@ -526,8 +533,12 @@
         <f>FV(A2, B2, , D2)</f>
         <v>1276.2815625000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(F2)</f>
+        <v>=FV(A2, B2, , D2)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.1</v>
       </c>
@@ -543,8 +554,12 @@
         <f>FV(A3/12, B3, C3)</f>
         <v>417.81821090259211</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H6" ca="1" si="0">_xlfn.FORMULATEXT(F3)</f>
+        <v>=FV(A3/12, B3, C3)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.1</v>
       </c>
@@ -562,8 +577,12 @@
         <f>FV(A4/12, B4, C4,, E4)</f>
         <v>417.81821090259211</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=FV(A4/12, B4, C4,, E4)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.1</v>
       </c>
@@ -581,8 +600,12 @@
         <f>FV(A5/12, B5, C5,, E5)</f>
         <v>421.30002932678042</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=FV(A5/12, B5, C5,, E5)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -592,8 +615,12 @@
         <f>FV(0.0042, 12, -1000, -10000, FALSE)</f>
         <v>22796.92466550941</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=FV(0.0042, 12, -1000, -10000, FALSE)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -601,7 +628,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update fv files (#162)
* Files updated for FV function documentation.

* Further FV changes
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/FV.xlsx
+++ b/xlsx/tests/docs/FV.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\Function descriptions\FV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FC729A-6FC1-4226-B328-4D36184339E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F210B7-B56C-4195-A32E-F8D7A39512E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{485CA009-6F4A-460D-891C-D7B8869F48AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>rate</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Future Value</t>
+  </si>
+  <si>
+    <t>Formula Text</t>
   </si>
 </sst>
 </file>
@@ -478,19 +481,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698A441E-9203-46F3-91E3-D681B30E39C3}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,8 +513,11 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>0.05</v>
       </c>
@@ -523,11 +530,15 @@
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="8">
-        <f>FV(A2, B2, , D2)</f>
+        <f>FV(A2,B2,,D2)</f>
         <v>1276.2815625000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(F2)</f>
+        <v>=FV(A2,B2,,D2)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.1</v>
       </c>
@@ -540,11 +551,15 @@
       <c r="D3" s="11"/>
       <c r="E3" s="10"/>
       <c r="F3" s="8">
-        <f>FV(A3/12, B3, C3)</f>
+        <f>FV(A3/12,B3,C3)</f>
         <v>417.81821090259211</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H6" ca="1" si="0">_xlfn.FORMULATEXT(F3)</f>
+        <v>=FV(A3/12,B3,C3)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.1</v>
       </c>
@@ -559,11 +574,15 @@
         <v>0</v>
       </c>
       <c r="F4" s="8">
-        <f>FV(A4/12, B4, C4,, E4)</f>
+        <f>FV(A4/12,B4,C4,,E4)</f>
         <v>417.81821090259211</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=FV(A4/12,B4,C4,,E4)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.1</v>
       </c>
@@ -578,22 +597,30 @@
         <v>1</v>
       </c>
       <c r="F5" s="8">
-        <f>FV(A5/12, B5, C5,, E5)</f>
+        <f>FV(A5/12,B5,C5,,E5)</f>
         <v>421.30002932678042</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=FV(A5/12,B5,C5,,E5)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="5"/>
       <c r="E6" s="2"/>
       <c r="F6" s="8">
-        <f>FV(0.0042, 12, -1000, -10000, FALSE)</f>
+        <f>FV(0.0042,12,-1000,-10000,FALSE)</f>
         <v>22796.92466550941</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=FV(0.0042,12,-1000,-10000,FALSE)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -601,7 +628,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to FV description and associated pages in the Features area.
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/FV.xlsx
+++ b/xlsx/tests/docs/FV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F210B7-B56C-4195-A32E-F8D7A39512E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94FB545-CB8A-42D7-89E1-9BBB777F61E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{485CA009-6F4A-460D-891C-D7B8869F48AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>rate</t>
   </si>
@@ -57,6 +57,73 @@
   </si>
   <si>
     <t>Formula Text</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Example of error propagation.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unable to convert </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> argument to a number.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unable to convert </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> argument to a Boolean.</t>
+    </r>
+  </si>
+  <si>
+    <t>Combination of valid inputs cause a #DIV/0! error. In this case, the formula for FV includes 1 divided by 0.</t>
+  </si>
+  <si>
+    <t>Combination of valid inputs cause a #NUM! error. In this case, the formula for FV includes the square root of -2.</t>
   </si>
 </sst>
 </file>
@@ -68,7 +135,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;\-[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +145,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -111,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,6 +222,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698A441E-9203-46F3-91E3-D681B30E39C3}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +575,7 @@
     <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>0.05</v>
       </c>
@@ -538,7 +619,7 @@
         <v>=FV(A2,B2,,D2)</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.1</v>
       </c>
@@ -559,7 +640,7 @@
         <v>=FV(A3/12,B3,C3)</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.1</v>
       </c>
@@ -582,7 +663,7 @@
         <v>=FV(A4/12,B4,C4,,E4)</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.1</v>
       </c>
@@ -605,7 +686,7 @@
         <v>=FV(A5/12,B5,C5,,E5)</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -620,7 +701,7 @@
         <v>=FV(0.0042,12,-1000,-10000,FALSE)</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -628,10 +709,125 @@
       <c r="E7" s="2"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="e">
+        <f>FV(SQRT(-1),2,3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B10" s="13" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A10)</f>
+        <v>=FV(SQRT(-1),2,3)</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="e">
+        <f>FV("str",2,3,4,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B11" s="13" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A11)</f>
+        <v>=FV("str",2,3,4,TRUE)</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="e">
+        <f>FV(1,2,3,4,"false")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B12" s="13" t="str">
+        <f t="shared" ref="B12:B14" ca="1" si="1">_xlfn.FORMULATEXT(A12)</f>
+        <v>=FV(1,2,3,4,"false")</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="e">
+        <f>FV(-3,0.5,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B13" s="13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=FV(-3,0.5,1)</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="e">
+        <f>FV(-1,-1,1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=FV(-1,-1,1)</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="D14:J14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>